<commit_message>
Adding documentation on functions
</commit_message>
<xml_diff>
--- a/functions_list.xlsx
+++ b/functions_list.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmorley\OneDrive - Department for Education\Documents\Projects\qa_log_app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/thomas_morley_education_gov_uk/Documents/Documents/Projects/qa_log_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F84A2F59-0AD4-465A-9939-0D5212D844F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="160" documentId="8_{F84A2F59-0AD4-465A-9939-0D5212D844F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8E5138B-4934-4DBF-9BFE-56094433CE0E}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2790" windowWidth="29040" windowHeight="15840" xr2:uid="{A59CF254-4986-4C78-AF86-EFF68954D462}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{A59CF254-4986-4C78-AF86-EFF68954D462}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="functions.R" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="112">
   <si>
     <t>List of functions</t>
   </si>
@@ -97,6 +97,285 @@
   </si>
   <si>
     <t>Saves scores and comments to QA_checks SQL database (unless the row is empty in which case nothing happens). Also adds history rows to QA_checks_SCD</t>
+  </si>
+  <si>
+    <t>Arguments</t>
+  </si>
+  <si>
+    <t>observe_logtype</t>
+  </si>
+  <si>
+    <t>create_actionbutton</t>
+  </si>
+  <si>
+    <t>Log type and log type name, session, list of types, next tab list</t>
+  </si>
+  <si>
+    <t>Observes the log button being pressed and calls create_log</t>
+  </si>
+  <si>
+    <t>Log type, session, list of types, next tab list</t>
+  </si>
+  <si>
+    <t>Create action buttons for different types of log</t>
+  </si>
+  <si>
+    <t>Log type</t>
+  </si>
+  <si>
+    <t>Check rating number</t>
+  </si>
+  <si>
+    <t>Check id, session, list of qa checks</t>
+  </si>
+  <si>
+    <t>Check id, session</t>
+  </si>
+  <si>
+    <t>Query sentence, InList</t>
+  </si>
+  <si>
+    <t>Check rating input</t>
+  </si>
+  <si>
+    <t>Check id, dataframe of inputs from app, inputs from SQL, project id, SQL database name, connection, current time</t>
+  </si>
+  <si>
+    <t>individualChecks</t>
+  </si>
+  <si>
+    <t>Pulls in info from SQL on individual checks and inserts dummy info where there exists no data for that check</t>
+  </si>
+  <si>
+    <t>check id, dataframe of inputs from SQL</t>
+  </si>
+  <si>
+    <t>Functions for calculating scores</t>
+  </si>
+  <si>
+    <t>calculate_score</t>
+  </si>
+  <si>
+    <t>Check id</t>
+  </si>
+  <si>
+    <t>Converts word score to percentage scores, i.e. "1) Excellent" -&gt; 100</t>
+  </si>
+  <si>
+    <t>iszero</t>
+  </si>
+  <si>
+    <t>Determines whether check has been completed or not (those marked N/A or TO BE CHECKED are then not taken into account in calculation of averages)</t>
+  </si>
+  <si>
+    <t>scoresfunc</t>
+  </si>
+  <si>
+    <t>List of checks</t>
+  </si>
+  <si>
+    <t>Applies calculate_score to all checks and then calculates percentage for each pillar</t>
+  </si>
+  <si>
+    <t>scorecolours</t>
+  </si>
+  <si>
+    <t>Percentage of pillar</t>
+  </si>
+  <si>
+    <t>Determines colour of text box depending on percentage score of each pillar</t>
+  </si>
+  <si>
+    <t>Functions for displaying extra info on checks</t>
+  </si>
+  <si>
+    <t>observe_info</t>
+  </si>
+  <si>
+    <t>Check id, list of log types</t>
+  </si>
+  <si>
+    <t>Creates modal to display extra info on each check, with text specific for the type of log</t>
+  </si>
+  <si>
+    <t>tooltip_ui_render</t>
+  </si>
+  <si>
+    <t>Creates tooltips for each check, with text specific for the type of log</t>
+  </si>
+  <si>
+    <t>Functions for error messages</t>
+  </si>
+  <si>
+    <t>check_mandatory</t>
+  </si>
+  <si>
+    <t>Check id, list of log types, list of check names</t>
+  </si>
+  <si>
+    <t>check_NA_mandatory</t>
+  </si>
+  <si>
+    <t>Determines whether a mandatory check has been marked "N/A"</t>
+  </si>
+  <si>
+    <t>Determines whether a mandatory check has been marked "TO BE CHECKED"</t>
+  </si>
+  <si>
+    <t>check_significant</t>
+  </si>
+  <si>
+    <t>Determines whether a check has been marked "5) Significant issues"</t>
+  </si>
+  <si>
+    <t>Functions for reading in historical records</t>
+  </si>
+  <si>
+    <t>select_old_log</t>
+  </si>
+  <si>
+    <t>Selected date, project ID</t>
+  </si>
+  <si>
+    <t>read_old_log</t>
+  </si>
+  <si>
+    <t>Calls select_old_log, and then selects entry closest to selected date (or if there doesn't exist any entry, reads in current data)</t>
+  </si>
+  <si>
+    <t>Reads in all records of log info from SCD table saved since selected date for relevant project ID</t>
+  </si>
+  <si>
+    <t>Calls read_old_log, and then builds UI for preview of log info line</t>
+  </si>
+  <si>
+    <t>displayingoldlog</t>
+  </si>
+  <si>
+    <t>select_old_check</t>
+  </si>
+  <si>
+    <t>Check id, selected date, project id</t>
+  </si>
+  <si>
+    <t>Reads in all records of check info from SCD table saved since selected date for relevant project id and check id</t>
+  </si>
+  <si>
+    <t>read_old_check</t>
+  </si>
+  <si>
+    <t>Calls select_old_check, and then selects entry closest to select date (or if there doesn't exist any entry, reads in current data)</t>
+  </si>
+  <si>
+    <t>displayingoldchecks</t>
+  </si>
+  <si>
+    <t>Check id, selected date, project id, types list, check names dataframe</t>
+  </si>
+  <si>
+    <t>Calls read_old_check, and builds ui for each individual check to be displayed in the preview pane</t>
+  </si>
+  <si>
+    <t>checkscorehistory</t>
+  </si>
+  <si>
+    <t>zeroscorehistory</t>
+  </si>
+  <si>
+    <t>Calls read_old_check, and then determines whether check has been completed or not, to allow us to calculate overall pillar percentages in preview pane</t>
+  </si>
+  <si>
+    <t>Calls read_old_check, and then determines a percentage score for each check to allow us to calculate overall pillar percentages in preview pane</t>
+  </si>
+  <si>
+    <t>weightings_old</t>
+  </si>
+  <si>
+    <t>Calls read_old_log, and then splits the weightings string into separate weightings for each pillar</t>
+  </si>
+  <si>
+    <t>restore_log</t>
+  </si>
+  <si>
+    <t>Session, selected date, project ID</t>
+  </si>
+  <si>
+    <t>Calls read_old_log and updates log info row with old data</t>
+  </si>
+  <si>
+    <t>restore_checks</t>
+  </si>
+  <si>
+    <t>Session, check ID, selected date, project id</t>
+  </si>
+  <si>
+    <t>Calls read_old_check and then updates individual checks with old data</t>
+  </si>
+  <si>
+    <t>How is function used?</t>
+  </si>
+  <si>
+    <t>Called within observe_logtype function</t>
+  </si>
+  <si>
+    <t>functions.R</t>
+  </si>
+  <si>
+    <t>Applied across all types of log, to observe any of the "Create log" buttons being pressed</t>
+  </si>
+  <si>
+    <t>home_server.R</t>
+  </si>
+  <si>
+    <t>Called within out$newPanel to create an action button for each type of log. Applied across all log types</t>
+  </si>
+  <si>
+    <t>1. Called within update_checks function to read score from SQL
+2. Called within displayingoldchecks function to read previous scores from SQL SCD table
+3. Called within zeroscorehistory function to allow us to check whether ratings in SCD table were completed or not
+4. Called within restore_checks function to replace current check scores with previous scores</t>
+  </si>
+  <si>
+    <t>Called after observing "Submit project id", if the project id is valid. Run across all check ids relevant to log type</t>
+  </si>
+  <si>
+    <t>Used when observing "Back to home" (if there are no unsaved changes) or when observing "Definitely go back" (if there are unsaved changes)</t>
+  </si>
+  <si>
+    <t>main_server.R</t>
+  </si>
+  <si>
+    <t>Called within paste_other_input to save scores to SQL as numbers</t>
+  </si>
+  <si>
+    <t>Called when the save button is pressed. Applied across all check ids relevant to selected log type</t>
+  </si>
+  <si>
+    <t>1. Called to read in current check info from SQL for comparison against app inputs (so that it can display an "unsaved changes" warning message if they don't match).
+2. Called again upon each save for a similar purpose</t>
+  </si>
+  <si>
+    <t>Called within scoresfunc to allow us to calculate overall % scores for pillars</t>
+  </si>
+  <si>
+    <t>1. Called for each pillar to calculate overall pillar %
+2. Called within scorecolours to calculate colour of textbox displaying pillar %
+3. Called to calculate total % over all pillars</t>
+  </si>
+  <si>
+    <t>Called for each pillar to calculate colour of textbox displaying pillar %</t>
+  </si>
+  <si>
+    <t>Applied to all QA checks</t>
+  </si>
+  <si>
+    <t>Applied to all QA checks relevant to log type to get a list of how many are marked "TO BE CHECKED", and displays error if number is more than 0</t>
+  </si>
+  <si>
+    <t>Applied to all QA checks relevant to log type to get a list of how many are marked "N/A", and displays error if number is more than 0</t>
+  </si>
+  <si>
+    <t>Applied to all QA checks relevant to log type to get a list of how many are marked "5) Significant issues", and displays error if number is more than 0</t>
   </si>
 </sst>
 </file>
@@ -128,15 +407,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -144,20 +429,132 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,107 +869,568 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37DFAFE0-2B81-4786-94DE-4716B62530C7}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="33.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.86328125" customWidth="1"/>
+    <col min="2" max="2" width="16.86328125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="33.265625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="33.19921875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="B1" s="3"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" s="12" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B4" s="14"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="16"/>
+    </row>
+    <row r="5" spans="1:5" ht="72.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="D5" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="72.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="72.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" s="13" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B8" s="14"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="18"/>
+    </row>
+    <row r="9" spans="1:5" ht="99.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="D9" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="D10" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+      <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="D11" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12" s="13" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B12" s="14"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="18"/>
+    </row>
+    <row r="13" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B13" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="D13" s="5"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B14" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="D14" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="A15" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>20</v>
       </c>
+      <c r="D15" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="A16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A17" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="18"/>
+    </row>
+    <row r="18" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+      <c r="A19" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A20" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A21" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A22" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="18"/>
+    </row>
+    <row r="23" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A23" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A24" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A25" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="18"/>
+    </row>
+    <row r="26" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+      <c r="A26" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+      <c r="A27" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+      <c r="A28" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A29" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="18"/>
+    </row>
+    <row r="30" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A30" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30" s="5"/>
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+      <c r="A31" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A32" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D32" s="5"/>
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A33" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D33" s="5"/>
+      <c r="E33" s="6"/>
+    </row>
+    <row r="34" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+      <c r="A34" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D34" s="5"/>
+      <c r="E34" s="6"/>
+    </row>
+    <row r="35" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+      <c r="A35" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D35" s="5"/>
+      <c r="E35" s="6"/>
+    </row>
+    <row r="36" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+      <c r="A36" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D36" s="5"/>
+      <c r="E36" s="6"/>
+    </row>
+    <row r="37" spans="1:5" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A37" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D37" s="5"/>
+      <c r="E37" s="6"/>
+    </row>
+    <row r="38" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A38" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D38" s="5"/>
+      <c r="E38" s="6"/>
+    </row>
+    <row r="39" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A39" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D39" s="5"/>
+      <c r="E39" s="6"/>
+    </row>
+    <row r="40" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A40" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D40" s="8"/>
+      <c r="E40" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>